<commit_message>
Creación de query para inserts en compromisos
</commit_message>
<xml_diff>
--- a/downloads/12345678908/jdelgadob-plantilla.xlsx
+++ b/downloads/12345678908/jdelgadob-plantilla.xlsx
@@ -6,6 +6,19 @@
   <sheets>
     <sheet sheetId="1" name="Compromisos" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="nrocorrelativo">Compromisos!$A$1:$A$2</definedName>
+    <definedName name="origencompromiso">Compromisos!$B$1:$B$2</definedName>
+    <definedName name="seccion">Compromisos!$C$1:$C$2</definedName>
+    <definedName name="pagina">Compromisos!$D$1:$D$2</definedName>
+    <definedName name="contorigcomp">Compromisos!$E$1:$E$2</definedName>
+    <definedName name="resumen">Compromisos!$F$1:$F$2</definedName>
+    <definedName name="fechainicio">Compromisos!$G$1:$G$2</definedName>
+    <definedName name="construccion">Compromisos!$H$1:$H$2</definedName>
+    <definedName name="operacion">Compromisos!$I$1:$I$2</definedName>
+    <definedName name="cierre">Compromisos!$J$1:$J$2</definedName>
+    <definedName name="postcierre">Compromisos!$K$1:$K$2</definedName>
+  </definedNames>
   <calcPr calcId="171027"/>
 </workbook>
 </file>

</xml_diff>

<commit_message>
Se culminó con la carga masiva de compromisos
</commit_message>
<xml_diff>
--- a/downloads/12345678908/jdelgadob-plantilla.xlsx
+++ b/downloads/12345678908/jdelgadob-plantilla.xlsx
@@ -8,58 +8,54 @@
   </sheets>
   <definedNames>
     <definedName name="nrocorrelativo">Compromisos!$A$1:$A$2</definedName>
-    <definedName name="origencompromiso">Compromisos!$B$1:$B$2</definedName>
-    <definedName name="codigoglobal">Compromisos!$C$1:$C$2</definedName>
+    <definedName name="codigoglobal">Compromisos!$B$1:$B$2</definedName>
+    <definedName name="capitulo">Compromisos!$C$1:$C$2</definedName>
     <definedName name="seccion">Compromisos!$D$1:$D$2</definedName>
     <definedName name="pagina">Compromisos!$E$1:$E$2</definedName>
-    <definedName name="aspambasoc">Compromisos!$F$1:$F$2</definedName>
-    <definedName name="contorigcomp">Compromisos!$G$1:$G$2</definedName>
-    <definedName name="nombrerevisor">Compromisos!$H$1:$H$2</definedName>
-    <definedName name="comentarios">Compromisos!$I$1:$I$2</definedName>
-    <definedName name="operacion">Compromisos!$J$1:$J$2</definedName>
-    <definedName name="cierre">Compromisos!$K$1:$K$2</definedName>
+    <definedName name="temporalidad">Compromisos!$F$1:$F$2</definedName>
+    <definedName name="fechainicio">Compromisos!$G$1:$G$2</definedName>
+    <definedName name="frecuencia">Compromisos!$H$1:$H$2</definedName>
+    <definedName name="criticidad">Compromisos!$I$1:$I$2</definedName>
+    <definedName name="estadocumplimiento">Compromisos!$J$1:$J$2</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>Matriz Integrada de Compromisos de la Unidad de null</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>Matriz Integrada de Compromisos de la Unidad de Multiunidad</t>
   </si>
   <si>
     <t>Número correlativo</t>
   </si>
   <si>
-    <t>Origen compromiso</t>
-  </si>
-  <si>
     <t>Código global</t>
   </si>
   <si>
+    <t>Capítulo</t>
+  </si>
+  <si>
     <t>Sección</t>
   </si>
   <si>
     <t>Página</t>
   </si>
   <si>
-    <t>Aspecto asociado</t>
-  </si>
-  <si>
-    <t>Contenido original del compromiso</t>
-  </si>
-  <si>
-    <t>Nombre de revisor</t>
-  </si>
-  <si>
-    <t>Notas adicionales</t>
-  </si>
-  <si>
-    <t>Operación</t>
-  </si>
-  <si>
-    <t>Cierre</t>
+    <t>Temporalidad</t>
+  </si>
+  <si>
+    <t>Fecha de inicio</t>
+  </si>
+  <si>
+    <t>Frecuencia</t>
+  </si>
+  <si>
+    <t>Criticidad</t>
+  </si>
+  <si>
+    <t>Estado de cumplimiento</t>
   </si>
 </sst>
 </file>
@@ -446,13 +442,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:J2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="11" width="20" customWidth="1"/>
+    <col min="1" max="10" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -465,9 +461,8 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -497,14 +492,11 @@
       </c>
       <c r="J2" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>